<commit_message>
Motion detector rule template now uses brightness sensor
</commit_message>
<xml_diff>
--- a/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/ruletemplates/motion-template-data.xlsx
+++ b/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/ruletemplates/motion-template-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dandrid\smarthome-cep-demonstrator\runtime\com.incquerylabs.smarthome.droolsbundle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dandrid\smarthome-cep-demonstrator\demo\com.incquerylabs.smarthome.demorules.homeio\src\main\resources\ruletemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>B_Motion_Detector</t>
   </si>
@@ -66,6 +66,33 @@
   </si>
   <si>
     <t>F_Lights_2_Analog</t>
+  </si>
+  <si>
+    <t>Brightness sensor</t>
+  </si>
+  <si>
+    <t>A_Brightness_Sensor</t>
+  </si>
+  <si>
+    <t>B_Brightness_Sensor</t>
+  </si>
+  <si>
+    <t>D_Brightness_Sensor</t>
+  </si>
+  <si>
+    <t>E_Brightness_Sensor</t>
+  </si>
+  <si>
+    <t>F_Brightness_Sensor</t>
+  </si>
+  <si>
+    <t>G_Brightness_Sensor</t>
+  </si>
+  <si>
+    <t>D_Lights_2_Analog</t>
+  </si>
+  <si>
+    <t>F_Lights_1_Analog</t>
   </si>
 </sst>
 </file>
@@ -407,13 +434,13 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
   </cols>
@@ -423,6 +450,9 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="3"/>
@@ -431,7 +461,10 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
@@ -440,7 +473,10 @@
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="1"/>
@@ -449,46 +485,67 @@
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>

</xml_diff>

<commit_message>
Roller shades rule refactor
</commit_message>
<xml_diff>
--- a/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/ruletemplates/motion-template-data.xlsx
+++ b/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/ruletemplates/motion-template-data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>B_Motion_Detector</t>
   </si>
@@ -59,12 +59,6 @@
     <t>F_Motion_Detector</t>
   </si>
   <si>
-    <t>G_Lights_Analog</t>
-  </si>
-  <si>
-    <t>G_Motion_Detector</t>
-  </si>
-  <si>
     <t>F_Lights_2_Analog</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
   </si>
   <si>
     <t>F_Brightness_Sensor</t>
-  </si>
-  <si>
-    <t>G_Brightness_Sensor</t>
   </si>
   <si>
     <t>D_Lights_2_Analog</t>
@@ -450,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -462,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
@@ -474,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
@@ -486,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>6</v>
@@ -497,10 +488,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -508,7 +499,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
@@ -519,10 +510,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,22 +521,15 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="A9" s="4"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>

</xml_diff>